<commit_message>
Updated processing of scenario data and output format. Both linear and shiny forms functional.
</commit_message>
<xml_diff>
--- a/injuries/input_injuries.xlsx
+++ b/injuries/input_injuries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -451,6 +451,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -535,12 +536,13 @@
   <dimension ref="A1:BG86"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,7 +1619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>35</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>38</v>
       </c>
@@ -1975,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>39</v>
       </c>
@@ -2154,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>40</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>46</v>
       </c>

</xml_diff>